<commit_message>
GDD + Mechanics aktualisiert
</commit_message>
<xml_diff>
--- a/_WIP/Tobias/Mechanics.xlsx
+++ b/_WIP/Tobias/Mechanics.xlsx
@@ -21,7 +21,7 @@
     <author>Tobias Schuster</author>
   </authors>
   <commentList>
-    <comment ref="B10" authorId="0">
+    <comment ref="B16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t>NO CASE</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
@@ -208,7 +211,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,12 +232,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -248,12 +245,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,9 +283,7 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -303,9 +292,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -316,9 +303,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -328,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -339,20 +324,41 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -360,6 +366,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:F16" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A2:F16"/>
+  <sortState ref="A3:F16">
+    <sortCondition ref="A2:A16"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Category"/>
+    <tableColumn id="2" name="Mechanic"/>
+    <tableColumn id="3" name="Preference"/>
+    <tableColumn id="4" name="Prio"/>
+    <tableColumn id="5" name="Complexity"/>
+    <tableColumn id="6" name="Risk"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -652,246 +676,325 @@
   <dimension ref="A2:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" customWidth="1"/>
-    <col min="3" max="6" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="12" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="7">
+        <v>3</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="8">
+        <v>3</v>
+      </c>
+      <c r="F6" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="7">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="E9" s="9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="6">
+        <v>21</v>
+      </c>
+      <c r="F10" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="9">
+        <v>3</v>
+      </c>
+      <c r="F11" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="D12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="8">
+        <v>8</v>
+      </c>
+      <c r="F12" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="B13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="14" t="s">
+      <c r="E13" s="8">
+        <v>5</v>
+      </c>
+      <c r="F13" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="E14" s="8">
+        <v>8</v>
+      </c>
+      <c r="F14" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="8">
+        <v>13</v>
+      </c>
+      <c r="F15" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="14" t="s">
+      <c r="D16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
+      <c r="E16" s="8">
+        <v>5</v>
+      </c>
+      <c r="F16" s="8">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>